<commit_message>
Existing API updated with latest payload
</commit_message>
<xml_diff>
--- a/otp/otpPayload.xlsx
+++ b/otp/otpPayload.xlsx
@@ -548,7 +548,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>64eb8e992d38070001be7059</t>
+          <t>{"timestamp":1724397723556,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -579,7 +579,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>64eb8e993fa91400012a3963</t>
+          <t>{"timestamp":1724397723788,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -622,7 +622,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>64eb8e9a2d38070001be705a</t>
+          <t>{"timestamp":1724397724043,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -665,7 +665,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>64eb8e9b3fa91400012a3964</t>
+          <t>{"timestamp":1724397724265,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -708,7 +708,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>64eb8e9c3fa91400012a3965</t>
+          <t>{"timestamp":1724397724512,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -751,7 +751,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159069049,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159069},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397724703,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -794,7 +794,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>64eb8e9d3fa91400012a3966</t>
+          <t>{"timestamp":1724397724974,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -837,7 +837,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>64eb8e9e2d38070001be705b</t>
+          <t>{"timestamp":1724397725220,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -880,7 +880,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>64eb8e9f3fa91400012a3967</t>
+          <t>{"timestamp":1724397725469,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -923,7 +923,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>64eb8ea02d38070001be705c</t>
+          <t>{"timestamp":1724397725649,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -966,7 +966,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>64eb8ea12d38070001be705d</t>
+          <t>{"timestamp":1724397725926,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>64eb8ea13fa91400012a3968</t>
+          <t>{"timestamp":1724397726123,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>64eb8ea22d38070001be705e</t>
+          <t>{"timestamp":1724397726306,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159075567,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159075},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397726568,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>64eb8ea42d38070001be705f</t>
+          <t>{"timestamp":1724397726900,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159077428,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159077},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397727174,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>64eb8ea63fa91400012a3969</t>
+          <t>{"timestamp":1724397727417,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>64eb8ea72d38070001be7060</t>
+          <t>{"timestamp":1724397727622,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>64eb8ea83fa91400012a396a</t>
+          <t>{"timestamp":1724397727906,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159081214,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159081},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397728125,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>64eb8ea92d38070001be7061</t>
+          <t>{"timestamp":1724397728275,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>64eb8eaa3fa91400012a396b</t>
+          <t>{"timestamp":1724397728522,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>64eb8eab2d38070001be7062</t>
+          <t>{"timestamp":1724397728712,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>64eb8eac3fa91400012a396c</t>
+          <t>{"timestamp":1724397728932,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>64eb8ead2d38070001be7063</t>
+          <t>{"timestamp":1724397729425,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>64eb8eae3fa91400012a396d</t>
+          <t>{"timestamp":1724397729746,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>64eb8eaf3fa91400012a396e</t>
+          <t>{"timestamp":1724397730063,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>64eb8eaf2d38070001be7064</t>
+          <t>{"timestamp":1724397730310,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>64eb8eb03fa91400012a396f</t>
+          <t>{"timestamp":1724397730879,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>64eb8eb12d38070001be7065</t>
+          <t>{"timestamp":1724397731355,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>64eb8eb23fa91400012a3970</t>
+          <t>{"timestamp":1724397731698,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>64eb8eb32d38070001be7066</t>
+          <t>{"timestamp":1724397731905,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>64eb8eb42d38070001be7067</t>
+          <t>{"timestamp":1724397732174,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>64eb8eb53fa91400012a3971</t>
+          <t>{"timestamp":1724397732800,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>64eb8eb52d38070001be7068</t>
+          <t>{"timestamp":1724397733048,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>64eb8eb63fa91400012a3972</t>
+          <t>{"timestamp":1724397733338,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>64eb8eb73fa91400012a3973</t>
+          <t>{"timestamp":1724397733619,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>64eb8eb82d38070001be7069</t>
+          <t>{"timestamp":1724397733978,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
@@ -2170,7 +2170,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>64eb8eb92d38070001be706a</t>
+          <t>{"timestamp":1724397734192,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>64eb8eba3fa91400012a3974</t>
+          <t>{"timestamp":1724397734837,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>64eb8ebb3fa91400012a3975</t>
+          <t>{"timestamp":1724397735678,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -2287,7 +2287,7 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159099955,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159099},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397736056,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
@@ -2322,7 +2322,7 @@
       <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159100876,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159100},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397736658,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -2357,7 +2357,7 @@
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159101741,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159101},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397742534,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -2392,7 +2392,7 @@
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159102514,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159102},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397743518,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -2427,7 +2427,7 @@
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159103438,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159103},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397743923,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -2462,7 +2462,7 @@
       <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159104355,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159104},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397744337,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -2497,7 +2497,7 @@
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159105280,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159105},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397744884,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -2532,7 +2532,7 @@
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159106157,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159106},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397745316,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -2567,7 +2567,7 @@
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159107025,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159107},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397745627,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -2602,7 +2602,7 @@
       <c r="A52" t="inlineStr"/>
       <c r="B52" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159107943,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159107},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397746597,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -2637,7 +2637,7 @@
       <c r="A53" t="inlineStr"/>
       <c r="B53" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159108882,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159108},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397746872,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -2672,7 +2672,7 @@
       <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159109694,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159109},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397747222,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
@@ -2707,7 +2707,7 @@
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159110511,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159110},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397747538,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
@@ -2742,7 +2742,7 @@
       <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159111554,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159111},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397747936,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
@@ -2777,7 +2777,7 @@
       <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159112467,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159112},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397748441,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
@@ -2812,7 +2812,7 @@
       <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159113424,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159113},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397748769,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
@@ -2847,7 +2847,7 @@
       <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159114202,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159114},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397749070,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
@@ -2882,7 +2882,7 @@
       <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159115013,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159115},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397749357,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
@@ -2917,7 +2917,7 @@
       <c r="A61" t="inlineStr"/>
       <c r="B61" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159115929,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159115},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397750635,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
@@ -2952,7 +2952,7 @@
       <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159116849,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159116},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397751253,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
@@ -2987,7 +2987,7 @@
       <c r="A63" t="inlineStr"/>
       <c r="B63" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159117615,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159117},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397751817,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
@@ -3022,7 +3022,7 @@
       <c r="A64" t="inlineStr"/>
       <c r="B64" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159118397,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159118},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397752389,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
@@ -3057,7 +3057,7 @@
       <c r="A65" t="inlineStr"/>
       <c r="B65" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159119316,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159119},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397752825,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
@@ -3092,7 +3092,7 @@
       <c r="A66" t="inlineStr"/>
       <c r="B66" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159120180,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159120},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397753266,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
@@ -3127,7 +3127,7 @@
       <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr">
         <is>
-          <t>{"timestamp":1693159121076,"origin":"iam-service","errorCode":4005,"errorMessage":"OTP has been expired. Please request for a new OTP.","cause":{"message":"OTP has been expired. Please request for a new OTP.","timestamp":1693159121},"status":"BAD_REQUEST"}</t>
+          <t>{"timestamp":1724397753538,"origin":"mobius-iam-service","errorCode":400000,"errorMessage":"Field validation failed: constraint violation","cause":{"message":"Field validation failed: constraint violation","timestamp":0},"errorObject":{"userType":"userType must not be null or empty"},"httpStatusCode":"BAD_REQUEST"}</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>

</xml_diff>